<commit_message>
updated code and added extent report listener
</commit_message>
<xml_diff>
--- a/resources/Automation_Data.xlsx
+++ b/resources/Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pairaj01\eclipse-workspace\GmailTest\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A636CC0E-89BE-43DE-983E-E2A933FAE54F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21970449-CC38-485B-8B8A-292420A3604A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Gmail_Signup_Testdata" sheetId="1" r:id="rId1"/>
@@ -59,15 +59,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>January@2021</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -90,6 +81,15 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Peterson</t>
+  </si>
+  <si>
+    <t>January@2021#</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,16 +520,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -540,25 +540,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added gmail login test cases
</commit_message>
<xml_diff>
--- a/resources/Automation_Data.xlsx
+++ b/resources/Automation_Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pairaj01\eclipse-workspace\GmailTest\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21970449-CC38-485B-8B8A-292420A3604A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3FF35D-7435-4DBF-8C5C-98218CA8C883}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6BFA5E0A-9DDB-4471-A408-EA685EED7E6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Gmail_Signup_Testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Gmail_Signin_Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Scenario</t>
   </si>
@@ -90,6 +91,33 @@
   </si>
   <si>
     <t>January@2021#</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>6504603326</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>Vinayak</t>
+  </si>
+  <si>
+    <t>Naik</t>
+  </si>
+  <si>
+    <t>vinayaknaiktest1@gmail.com</t>
+  </si>
+  <si>
+    <t>January@123</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
   </si>
 </sst>
 </file>
@@ -127,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,12 +178,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +211,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3D2D7D-BAA5-4C81-81DB-F14C39826B7E}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,10 +546,12 @@
     <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.08984375" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="2"/>
+    <col min="6" max="9" width="8.7265625" style="2"/>
+    <col min="10" max="10" width="13.26953125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +579,11 @@
       <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -560,8 +611,11 @@
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -575,6 +629,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -583,4 +638,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1780B98-8677-4C13-8C40-48ED5F286163}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B7DF9EEA-9E34-41EA-938A-4732D6BC5D7D}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{585FD5EF-2B25-4A00-AF02-9E47B2F020D5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>